<commit_message>
Refactor focal length calculation script: streamline data loading and calculations, enhance readability, and improve output formatting.
</commit_message>
<xml_diff>
--- a/data/focal-length.xlsx
+++ b/data/focal-length.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuba-\Desktop\simple_graph_tool_xdf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2286F95E-AE07-4061-923D-579388BDA278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E4D8CF-3652-4329-BEC5-DF56B179D142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2475" yWindow="2940" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>x1</t>
   </si>
@@ -46,10 +46,10 @@
     <t>y</t>
   </si>
   <si>
-    <t>f</t>
+    <t>l</t>
   </si>
   <si>
-    <t>l</t>
+    <t>lp</t>
   </si>
 </sst>
 </file>
@@ -370,7 +370,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,39 +384,39 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>170</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>132</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>133</v>
-      </c>
-      <c r="D2">
-        <v>132.5</v>
       </c>
       <c r="E2">
         <v>132.5</v>
@@ -425,84 +425,96 @@
         <v>132.5</v>
       </c>
       <c r="G2">
+        <v>132.5</v>
+      </c>
+      <c r="H2">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>159</v>
-      </c>
-      <c r="B3">
-        <v>119</v>
       </c>
       <c r="C3">
         <v>119</v>
       </c>
       <c r="D3">
+        <v>119</v>
+      </c>
+      <c r="E3">
         <v>119.5</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>119</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>119.5</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>148</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>108.6</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>108</v>
-      </c>
-      <c r="D4">
-        <v>108.5</v>
       </c>
       <c r="E4">
         <v>108.5</v>
       </c>
       <c r="F4">
+        <v>108.5</v>
+      </c>
+      <c r="G4">
         <v>107.5</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>41.5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>137</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>94</v>
-      </c>
-      <c r="C5">
-        <v>93</v>
       </c>
       <c r="D5">
         <v>93</v>
       </c>
       <c r="E5">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5">
         <v>94</v>
       </c>
       <c r="G5">
+        <v>94</v>
+      </c>
+      <c r="H5">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>126</v>
-      </c>
-      <c r="B6">
-        <v>79</v>
       </c>
       <c r="C6">
         <v>79</v>
@@ -514,9 +526,12 @@
         <v>79</v>
       </c>
       <c r="F6">
+        <v>79</v>
+      </c>
+      <c r="G6">
         <v>78</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>48</v>
       </c>
     </row>
@@ -527,66 +542,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20638A32-2F78-4FF7-BE20-8093E416D153}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>170</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>38</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>39</v>
-      </c>
-      <c r="D2">
-        <v>38.5</v>
       </c>
       <c r="E2">
         <v>38.5</v>
       </c>
       <c r="F2">
+        <v>38.5</v>
+      </c>
+      <c r="G2">
         <v>39</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>159</v>
-      </c>
-      <c r="B3">
-        <v>40</v>
       </c>
       <c r="C3">
         <v>40</v>
@@ -601,41 +622,47 @@
         <v>40</v>
       </c>
       <c r="G3">
+        <v>40</v>
+      </c>
+      <c r="H3">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>148</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>40.5</v>
-      </c>
-      <c r="C4">
-        <v>41</v>
       </c>
       <c r="D4">
         <v>41</v>
       </c>
       <c r="E4">
+        <v>41</v>
+      </c>
+      <c r="F4">
         <v>41.5</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>41</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>137</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>43</v>
-      </c>
-      <c r="C5">
-        <v>43.5</v>
       </c>
       <c r="D5">
         <v>43.5</v>
@@ -647,29 +674,35 @@
         <v>43.5</v>
       </c>
       <c r="G5">
+        <v>43.5</v>
+      </c>
+      <c r="H5">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>126</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>46</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>46.5</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>47.5</v>
-      </c>
-      <c r="E6">
-        <v>47</v>
       </c>
       <c r="F6">
         <v>47</v>
       </c>
       <c r="G6">
+        <v>47</v>
+      </c>
+      <c r="H6">
         <v>79</v>
       </c>
     </row>

</xml_diff>